<commit_message>
fixed import penerimaan motor
</commit_message>
<xml_diff>
--- a/excel_penerimaan_motor.xlsx
+++ b/excel_penerimaan_motor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="50">
   <si>
     <t>No Polisi</t>
   </si>
@@ -50,12 +50,6 @@
     <t>Warna</t>
   </si>
   <si>
-    <t>Kode Gudang</t>
-  </si>
-  <si>
-    <t>B08080VND</t>
-  </si>
-  <si>
     <t>SJ00854545</t>
   </si>
   <si>
@@ -75,6 +69,111 @@
   </si>
   <si>
     <t>2016-11-11</t>
+  </si>
+  <si>
+    <t>B08080VND1</t>
+  </si>
+  <si>
+    <t>B08080VND2</t>
+  </si>
+  <si>
+    <t>B08080VND3</t>
+  </si>
+  <si>
+    <t>B08080VND4</t>
+  </si>
+  <si>
+    <t>B08080VND5</t>
+  </si>
+  <si>
+    <t>B08080VND6</t>
+  </si>
+  <si>
+    <t>B08080VND7</t>
+  </si>
+  <si>
+    <t>B08080VND8</t>
+  </si>
+  <si>
+    <t>B08080VND9</t>
+  </si>
+  <si>
+    <t>B08080VND10</t>
+  </si>
+  <si>
+    <t>B08080VND11</t>
+  </si>
+  <si>
+    <t>B08080VND12</t>
+  </si>
+  <si>
+    <t>B08080VND13</t>
+  </si>
+  <si>
+    <t>B08080VND14</t>
+  </si>
+  <si>
+    <t>B08080VND15</t>
+  </si>
+  <si>
+    <t>B08080VND16</t>
+  </si>
+  <si>
+    <t>B08080VND17</t>
+  </si>
+  <si>
+    <t>B08080VND18</t>
+  </si>
+  <si>
+    <t>B08080VND19</t>
+  </si>
+  <si>
+    <t>B08080VND20</t>
+  </si>
+  <si>
+    <t>B08080VND21</t>
+  </si>
+  <si>
+    <t>B08080VND22</t>
+  </si>
+  <si>
+    <t>B08080VND23</t>
+  </si>
+  <si>
+    <t>B08080VND24</t>
+  </si>
+  <si>
+    <t>B08080VND25</t>
+  </si>
+  <si>
+    <t>B08080VND26</t>
+  </si>
+  <si>
+    <t>B08080VND27</t>
+  </si>
+  <si>
+    <t>B08080VND28</t>
+  </si>
+  <si>
+    <t>B08080VND29</t>
+  </si>
+  <si>
+    <t>B08080VND30</t>
+  </si>
+  <si>
+    <t>B08080VND31</t>
+  </si>
+  <si>
+    <t>B08080VND32</t>
+  </si>
+  <si>
+    <t>B08080VND33</t>
+  </si>
+  <si>
+    <t>B08080VND34</t>
+  </si>
+  <si>
+    <t>Kode Gudag</t>
   </si>
 </sst>
 </file>
@@ -435,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,35 +579,992 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2">
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" t="s">
+        <v>13</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" t="s">
+        <v>13</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" t="s">
+        <v>13</v>
+      </c>
+      <c r="I33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" t="s">
+        <v>13</v>
+      </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I35">
         <v>2</v>
       </c>
     </row>

</xml_diff>